<commit_message>
change string source file
</commit_message>
<xml_diff>
--- a/LanguageParser.xlsx
+++ b/LanguageParser.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukelin/Documents/WorkSpaceLuke/LanguageParser/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="270" yWindow="600" windowWidth="24615" windowHeight="11445"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Id</t>
   </si>
@@ -28,9 +41,6 @@
     <t>account_activating</t>
   </si>
   <si>
-    <t>Activation …</t>
-  </si>
-  <si>
     <t>account_activation_failed</t>
   </si>
   <si>
@@ -58,23 +68,35 @@
     <t>zh</t>
   </si>
   <si>
-    <t>激活</t>
-  </si>
-  <si>
     <t>激活未成功</t>
   </si>
   <si>
-    <t>Activating…%1$s</t>
-  </si>
-  <si>
-    <t>重试11</t>
+    <t>Activating…%S%</t>
+  </si>
+  <si>
+    <t>重试</t>
+  </si>
+  <si>
+    <t>Activation …%S%</t>
+  </si>
+  <si>
+    <t>激活%S%</t>
+  </si>
+  <si>
+    <t>account_info</t>
+  </si>
+  <si>
+    <t>Name is %S%, age is %D%</t>
+  </si>
+  <si>
+    <t>名字是%S%, 年龄是%D%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -170,6 +192,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -216,12 +243,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -248,14 +275,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -282,6 +310,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,22 +486,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.83203125" customWidth="1"/>
+    <col min="3" max="3" width="36.5" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -480,13 +509,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -511,7 +540,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1">
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -519,1322 +548,1336 @@
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>4</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1">
+    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1">
+    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1">
+    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1">
+    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1">
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1">
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="4:4" ht="15.75" customHeight="1">
+    <row r="17" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="4:4" ht="15.75" customHeight="1">
+    <row r="18" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="4:4" ht="15.75" customHeight="1">
+    <row r="19" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="4:4" ht="15.75" customHeight="1">
+    <row r="20" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="4:4" ht="15.75" customHeight="1">
+    <row r="21" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="4:4" ht="15.75" customHeight="1">
+    <row r="22" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="4:4" ht="15.75" customHeight="1">
+    <row r="23" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="4:4" ht="15.75" customHeight="1">
+    <row r="24" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="4:4" ht="15.75" customHeight="1">
+    <row r="25" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="4:4" ht="15.75" customHeight="1">
+    <row r="26" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="4:4" ht="15.75" customHeight="1">
+    <row r="27" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="4:4" ht="15.75" customHeight="1">
+    <row r="28" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="4:4" ht="15.75" customHeight="1">
+    <row r="29" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="4:4" ht="15.75" customHeight="1">
+    <row r="30" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="4:4" ht="15.75" customHeight="1">
+    <row r="31" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="4:4" ht="15.75" customHeight="1">
+    <row r="32" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="4:4" ht="15.75" customHeight="1">
+    <row r="33" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="4:4" ht="15.75" customHeight="1">
+    <row r="34" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="4:4" ht="15.75" customHeight="1">
+    <row r="35" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="4:4" ht="15.75" customHeight="1">
+    <row r="36" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="4:4" ht="15.75" customHeight="1">
+    <row r="37" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="4:4" ht="15.75" customHeight="1">
+    <row r="38" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="4:4" ht="15.75" customHeight="1">
+    <row r="39" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="4:4" ht="15.75" customHeight="1">
+    <row r="40" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="4:4" ht="15.75" customHeight="1">
+    <row r="41" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="4:4" ht="15.75" customHeight="1">
+    <row r="42" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="4:4" ht="15.75" customHeight="1">
+    <row r="43" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="4:4" ht="15.75" customHeight="1">
+    <row r="44" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="4:4" ht="15.75" customHeight="1">
+    <row r="45" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="4:4" ht="15.75" customHeight="1">
+    <row r="46" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="4:4" ht="15.75" customHeight="1">
+    <row r="47" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="4:4" ht="15.75" customHeight="1">
+    <row r="48" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="4:4" ht="15.75" customHeight="1">
+    <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="4:4" ht="15.75" customHeight="1">
+    <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="4:4" ht="15.75" customHeight="1">
+    <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="4:4" ht="15.75" customHeight="1">
+    <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="4:4" ht="15.75" customHeight="1">
+    <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="4:4" ht="15.75" customHeight="1">
+    <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="4:4" ht="15.75" customHeight="1">
+    <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="4:4" ht="15.75" customHeight="1">
+    <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="4:4" ht="15.75" customHeight="1">
+    <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="4:4" ht="15.75" customHeight="1">
+    <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="4:4" ht="15.75" customHeight="1">
+    <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="4:4" ht="15.75" customHeight="1">
+    <row r="60" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="4:4" ht="15.75" customHeight="1">
+    <row r="61" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="4:4" ht="15.75" customHeight="1">
+    <row r="62" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="4:4" ht="15.75" customHeight="1">
+    <row r="63" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="4:4" ht="15.75" customHeight="1">
+    <row r="64" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="4:4" ht="15.75" customHeight="1">
+    <row r="65" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="4:4" ht="15.75" customHeight="1">
+    <row r="66" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="4:4" ht="15.75" customHeight="1">
+    <row r="67" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="4:4" ht="15.75" customHeight="1">
+    <row r="68" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="4:4" ht="15.75" customHeight="1">
+    <row r="69" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="4:4" ht="15.75" customHeight="1">
+    <row r="70" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="4:4" ht="15.75" customHeight="1">
+    <row r="71" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="4:4" ht="15.75" customHeight="1">
+    <row r="72" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="4:4" ht="15.75" customHeight="1">
+    <row r="73" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="4:4" ht="15.75" customHeight="1">
+    <row r="74" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="4:4" ht="15.75" customHeight="1">
+    <row r="75" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="4:4" ht="15.75" customHeight="1">
+    <row r="76" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="4:4" ht="15.75" customHeight="1">
+    <row r="77" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="4:4" ht="15.75" customHeight="1">
+    <row r="78" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="4:4" ht="15.75" customHeight="1">
+    <row r="79" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="4:4" ht="15.75" customHeight="1">
+    <row r="80" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="4:4" ht="15.75" customHeight="1">
+    <row r="81" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="4:4" ht="15.75" customHeight="1">
+    <row r="82" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="4:4" ht="15.75" customHeight="1">
+    <row r="83" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="4:4" ht="15.75" customHeight="1">
+    <row r="84" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="4:4" ht="15.75" customHeight="1">
+    <row r="85" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="4:4" ht="15.75" customHeight="1">
+    <row r="86" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="4:4" ht="15.75" customHeight="1">
+    <row r="87" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="4:4" ht="15.75" customHeight="1">
+    <row r="88" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="4:4" ht="15.75" customHeight="1">
+    <row r="89" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="4:4" ht="15.75" customHeight="1">
+    <row r="90" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="4:4" ht="15.75" customHeight="1">
+    <row r="91" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="4:4" ht="15.75" customHeight="1">
+    <row r="92" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="4:4" ht="15.75" customHeight="1">
+    <row r="93" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="4:4" ht="15.75" customHeight="1">
+    <row r="94" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="4:4" ht="15.75" customHeight="1">
+    <row r="95" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="4:4" ht="15.75" customHeight="1">
+    <row r="96" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="4:4" ht="15.75" customHeight="1">
+    <row r="97" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="4:4" ht="15.75" customHeight="1">
+    <row r="98" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="4:4" ht="15.75" customHeight="1">
+    <row r="99" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="4:4" ht="15.75" customHeight="1">
+    <row r="100" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="4:4" ht="15.75" customHeight="1">
+    <row r="101" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="4:4" ht="15.75" customHeight="1">
+    <row r="102" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="4:4" ht="15.75" customHeight="1">
+    <row r="103" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="4:4" ht="15.75" customHeight="1">
+    <row r="104" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="4:4" ht="15.75" customHeight="1">
+    <row r="105" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="4:4" ht="15.75" customHeight="1">
+    <row r="106" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="4:4" ht="15.75" customHeight="1">
+    <row r="107" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="4:4" ht="15.75" customHeight="1">
+    <row r="108" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D108" s="3"/>
     </row>
-    <row r="109" spans="4:4" ht="15.75" customHeight="1">
+    <row r="109" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="4:4" ht="15.75" customHeight="1">
+    <row r="110" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="4:4" ht="15.75" customHeight="1">
+    <row r="111" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="4:4" ht="15.75" customHeight="1">
+    <row r="112" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D112" s="3"/>
     </row>
-    <row r="113" spans="4:4" ht="15.75" customHeight="1">
+    <row r="113" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="4:4" ht="15.75" customHeight="1">
+    <row r="114" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="4:4" ht="15.75" customHeight="1">
+    <row r="115" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="4:4" ht="15.75" customHeight="1">
+    <row r="116" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="4:4" ht="15.75" customHeight="1">
+    <row r="117" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="4:4" ht="15.75" customHeight="1">
+    <row r="118" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="4:4" ht="15.75" customHeight="1">
+    <row r="119" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="4:4" ht="15.75" customHeight="1">
+    <row r="120" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="4:4" ht="15.75" customHeight="1">
+    <row r="121" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="4:4" ht="15.75" customHeight="1">
+    <row r="122" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="4:4" ht="15.75" customHeight="1">
+    <row r="123" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="4:4" ht="15.75" customHeight="1">
+    <row r="124" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="4:4" ht="15.75" customHeight="1">
+    <row r="125" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="4:4" ht="15.75" customHeight="1">
+    <row r="126" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="4:4" ht="15.75" customHeight="1">
+    <row r="127" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="4:4" ht="15.75" customHeight="1">
+    <row r="128" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="4:4" ht="15.75" customHeight="1">
+    <row r="129" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D129" s="3"/>
     </row>
-    <row r="130" spans="4:4" ht="15.75" customHeight="1">
+    <row r="130" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="4:4" ht="15.75" customHeight="1">
+    <row r="131" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D131" s="3"/>
     </row>
-    <row r="132" spans="4:4" ht="15.75" customHeight="1">
+    <row r="132" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="4:4" ht="15.75" customHeight="1">
+    <row r="133" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D133" s="3"/>
     </row>
-    <row r="134" spans="4:4" ht="15.75" customHeight="1">
+    <row r="134" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="4:4" ht="15.75" customHeight="1">
+    <row r="135" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="4:4" ht="15.75" customHeight="1">
+    <row r="136" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="4:4" ht="15.75" customHeight="1">
+    <row r="137" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D137" s="3"/>
     </row>
-    <row r="138" spans="4:4" ht="15.75" customHeight="1">
+    <row r="138" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="4:4" ht="15.75" customHeight="1">
+    <row r="139" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="4:4" ht="15.75" customHeight="1">
+    <row r="140" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="4:4" ht="15.75" customHeight="1">
+    <row r="141" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="4:4" ht="15.75" customHeight="1">
+    <row r="142" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D142" s="3"/>
     </row>
-    <row r="143" spans="4:4" ht="15.75" customHeight="1">
+    <row r="143" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D143" s="3"/>
     </row>
-    <row r="144" spans="4:4" ht="15.75" customHeight="1">
+    <row r="144" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="4:4" ht="15.75" customHeight="1">
+    <row r="145" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="4:4" ht="15.75" customHeight="1">
+    <row r="146" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="4:4" ht="15.75" customHeight="1">
+    <row r="147" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="4:4" ht="15.75" customHeight="1">
+    <row r="148" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="4:4" ht="15.75" customHeight="1">
+    <row r="149" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="4:4" ht="15.75" customHeight="1">
+    <row r="150" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="4:4" ht="15.75" customHeight="1">
+    <row r="151" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D151" s="3"/>
     </row>
-    <row r="152" spans="4:4" ht="15.75" customHeight="1">
+    <row r="152" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D152" s="3"/>
     </row>
-    <row r="153" spans="4:4" ht="15.75" customHeight="1">
+    <row r="153" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D153" s="3"/>
     </row>
-    <row r="154" spans="4:4" ht="15.75" customHeight="1">
+    <row r="154" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D154" s="3"/>
     </row>
-    <row r="155" spans="4:4" ht="15.75" customHeight="1">
+    <row r="155" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D155" s="3"/>
     </row>
-    <row r="156" spans="4:4" ht="15.75" customHeight="1">
+    <row r="156" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D156" s="3"/>
     </row>
-    <row r="157" spans="4:4" ht="15.75" customHeight="1">
+    <row r="157" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D157" s="3"/>
     </row>
-    <row r="158" spans="4:4" ht="15.75" customHeight="1">
+    <row r="158" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D158" s="3"/>
     </row>
-    <row r="159" spans="4:4" ht="15.75" customHeight="1">
+    <row r="159" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D159" s="3"/>
     </row>
-    <row r="160" spans="4:4" ht="15.75" customHeight="1">
+    <row r="160" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D160" s="3"/>
     </row>
-    <row r="161" spans="4:4" ht="15.75" customHeight="1">
+    <row r="161" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D161" s="3"/>
     </row>
-    <row r="162" spans="4:4" ht="15.75" customHeight="1">
+    <row r="162" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D162" s="3"/>
     </row>
-    <row r="163" spans="4:4" ht="15.75" customHeight="1">
+    <row r="163" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D163" s="3"/>
     </row>
-    <row r="164" spans="4:4" ht="15.75" customHeight="1">
+    <row r="164" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D164" s="3"/>
     </row>
-    <row r="165" spans="4:4" ht="15.75" customHeight="1">
+    <row r="165" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D165" s="3"/>
     </row>
-    <row r="166" spans="4:4" ht="15.75" customHeight="1">
+    <row r="166" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D166" s="3"/>
     </row>
-    <row r="167" spans="4:4" ht="15.75" customHeight="1">
+    <row r="167" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D167" s="3"/>
     </row>
-    <row r="168" spans="4:4" ht="15.75" customHeight="1">
+    <row r="168" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D168" s="3"/>
     </row>
-    <row r="169" spans="4:4" ht="15.75" customHeight="1">
+    <row r="169" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D169" s="3"/>
     </row>
-    <row r="170" spans="4:4" ht="15.75" customHeight="1">
+    <row r="170" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D170" s="3"/>
     </row>
-    <row r="171" spans="4:4" ht="15.75" customHeight="1">
+    <row r="171" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D171" s="3"/>
     </row>
-    <row r="172" spans="4:4" ht="15.75" customHeight="1">
+    <row r="172" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D172" s="3"/>
     </row>
-    <row r="173" spans="4:4" ht="15.75" customHeight="1">
+    <row r="173" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D173" s="3"/>
     </row>
-    <row r="174" spans="4:4" ht="15.75" customHeight="1">
+    <row r="174" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D174" s="3"/>
     </row>
-    <row r="175" spans="4:4" ht="15.75" customHeight="1">
+    <row r="175" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D175" s="3"/>
     </row>
-    <row r="176" spans="4:4" ht="15.75" customHeight="1">
+    <row r="176" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D176" s="3"/>
     </row>
-    <row r="177" spans="4:4" ht="15.75" customHeight="1">
+    <row r="177" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D177" s="3"/>
     </row>
-    <row r="178" spans="4:4" ht="15.75" customHeight="1">
+    <row r="178" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D178" s="3"/>
     </row>
-    <row r="179" spans="4:4" ht="15.75" customHeight="1">
+    <row r="179" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D179" s="3"/>
     </row>
-    <row r="180" spans="4:4" ht="15.75" customHeight="1">
+    <row r="180" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D180" s="3"/>
     </row>
-    <row r="181" spans="4:4" ht="15.75" customHeight="1">
+    <row r="181" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D181" s="3"/>
     </row>
-    <row r="182" spans="4:4" ht="15.75" customHeight="1">
+    <row r="182" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D182" s="3"/>
     </row>
-    <row r="183" spans="4:4" ht="15.75" customHeight="1">
+    <row r="183" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D183" s="3"/>
     </row>
-    <row r="184" spans="4:4" ht="15.75" customHeight="1">
+    <row r="184" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D184" s="3"/>
     </row>
-    <row r="185" spans="4:4" ht="15.75" customHeight="1">
+    <row r="185" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D185" s="3"/>
     </row>
-    <row r="186" spans="4:4" ht="15.75" customHeight="1">
+    <row r="186" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D186" s="3"/>
     </row>
-    <row r="187" spans="4:4" ht="15.75" customHeight="1">
+    <row r="187" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D187" s="3"/>
     </row>
-    <row r="188" spans="4:4" ht="15.75" customHeight="1">
+    <row r="188" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D188" s="3"/>
     </row>
-    <row r="189" spans="4:4" ht="15.75" customHeight="1">
+    <row r="189" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D189" s="3"/>
     </row>
-    <row r="190" spans="4:4" ht="15.75" customHeight="1">
+    <row r="190" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D190" s="3"/>
     </row>
-    <row r="191" spans="4:4" ht="15.75" customHeight="1">
+    <row r="191" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D191" s="3"/>
     </row>
-    <row r="192" spans="4:4" ht="15.75" customHeight="1">
+    <row r="192" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D192" s="3"/>
     </row>
-    <row r="193" spans="4:4" ht="15.75" customHeight="1">
+    <row r="193" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D193" s="3"/>
     </row>
-    <row r="194" spans="4:4" ht="15.75" customHeight="1">
+    <row r="194" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D194" s="3"/>
     </row>
-    <row r="195" spans="4:4" ht="15.75" customHeight="1">
+    <row r="195" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D195" s="3"/>
     </row>
-    <row r="196" spans="4:4" ht="15.75" customHeight="1">
+    <row r="196" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D196" s="3"/>
     </row>
-    <row r="197" spans="4:4" ht="15.75" customHeight="1">
+    <row r="197" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D197" s="3"/>
     </row>
-    <row r="198" spans="4:4" ht="15.75" customHeight="1">
+    <row r="198" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D198" s="3"/>
     </row>
-    <row r="199" spans="4:4" ht="15.75" customHeight="1">
+    <row r="199" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D199" s="3"/>
     </row>
-    <row r="200" spans="4:4" ht="15.75" customHeight="1">
+    <row r="200" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D200" s="3"/>
     </row>
-    <row r="201" spans="4:4" ht="15.75" customHeight="1">
+    <row r="201" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="4:4" ht="15.75" customHeight="1">
+    <row r="202" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D202" s="3"/>
     </row>
-    <row r="203" spans="4:4" ht="15.75" customHeight="1">
+    <row r="203" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D203" s="3"/>
     </row>
-    <row r="204" spans="4:4" ht="15.75" customHeight="1">
+    <row r="204" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D204" s="3"/>
     </row>
-    <row r="205" spans="4:4" ht="15.75" customHeight="1">
+    <row r="205" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D205" s="3"/>
     </row>
-    <row r="206" spans="4:4" ht="15.75" customHeight="1">
+    <row r="206" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="4:4" ht="15.75" customHeight="1">
+    <row r="207" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D207" s="3"/>
     </row>
-    <row r="208" spans="4:4" ht="15.75" customHeight="1">
+    <row r="208" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D208" s="3"/>
     </row>
-    <row r="209" spans="4:4" ht="15.75" customHeight="1">
+    <row r="209" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D209" s="3"/>
     </row>
-    <row r="210" spans="4:4" ht="15.75" customHeight="1">
+    <row r="210" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D210" s="3"/>
     </row>
-    <row r="211" spans="4:4" ht="15.75" customHeight="1">
+    <row r="211" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D211" s="3"/>
     </row>
-    <row r="212" spans="4:4" ht="15.75" customHeight="1">
+    <row r="212" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D212" s="3"/>
     </row>
-    <row r="213" spans="4:4" ht="15.75" customHeight="1">
+    <row r="213" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D213" s="3"/>
     </row>
-    <row r="214" spans="4:4" ht="15.75" customHeight="1">
+    <row r="214" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="4:4" ht="15.75" customHeight="1">
+    <row r="215" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D215" s="3"/>
     </row>
-    <row r="216" spans="4:4" ht="15.75" customHeight="1">
+    <row r="216" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D216" s="3"/>
     </row>
-    <row r="217" spans="4:4" ht="15.75" customHeight="1">
+    <row r="217" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D217" s="3"/>
     </row>
-    <row r="218" spans="4:4" ht="15.75" customHeight="1">
+    <row r="218" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="4:4" ht="15.75" customHeight="1">
+    <row r="219" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D219" s="3"/>
     </row>
-    <row r="220" spans="4:4" ht="15.75" customHeight="1">
+    <row r="220" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D220" s="3"/>
     </row>
-    <row r="221" spans="4:4" ht="15.75" customHeight="1">
+    <row r="221" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D221" s="3"/>
     </row>
-    <row r="222" spans="4:4" ht="15.75" customHeight="1">
+    <row r="222" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D222" s="3"/>
     </row>
-    <row r="223" spans="4:4" ht="15.75" customHeight="1">
+    <row r="223" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D223" s="3"/>
     </row>
-    <row r="224" spans="4:4" ht="15.75" customHeight="1">
+    <row r="224" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D224" s="3"/>
     </row>
-    <row r="225" spans="4:4" ht="15.75" customHeight="1">
+    <row r="225" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D225" s="3"/>
     </row>
-    <row r="226" spans="4:4" ht="15.75" customHeight="1">
+    <row r="226" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D226" s="3"/>
     </row>
-    <row r="227" spans="4:4" ht="15.75" customHeight="1">
+    <row r="227" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D227" s="3"/>
     </row>
-    <row r="228" spans="4:4" ht="15.75" customHeight="1">
+    <row r="228" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D228" s="3"/>
     </row>
-    <row r="229" spans="4:4" ht="15.75" customHeight="1">
+    <row r="229" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D229" s="3"/>
     </row>
-    <row r="230" spans="4:4" ht="15.75" customHeight="1">
+    <row r="230" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D230" s="3"/>
     </row>
-    <row r="231" spans="4:4" ht="15.75" customHeight="1">
+    <row r="231" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D231" s="3"/>
     </row>
-    <row r="232" spans="4:4" ht="15.75" customHeight="1">
+    <row r="232" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D232" s="3"/>
     </row>
-    <row r="233" spans="4:4" ht="15.75" customHeight="1">
+    <row r="233" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D233" s="3"/>
     </row>
-    <row r="234" spans="4:4" ht="15.75" customHeight="1">
+    <row r="234" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D234" s="3"/>
     </row>
-    <row r="235" spans="4:4" ht="15.75" customHeight="1">
+    <row r="235" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D235" s="3"/>
     </row>
-    <row r="236" spans="4:4" ht="15.75" customHeight="1">
+    <row r="236" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D236" s="3"/>
     </row>
-    <row r="237" spans="4:4" ht="15.75" customHeight="1">
+    <row r="237" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D237" s="3"/>
     </row>
-    <row r="238" spans="4:4" ht="15.75" customHeight="1">
+    <row r="238" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D238" s="3"/>
     </row>
-    <row r="239" spans="4:4" ht="15.75" customHeight="1">
+    <row r="239" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D239" s="3"/>
     </row>
-    <row r="240" spans="4:4" ht="15.75" customHeight="1">
+    <row r="240" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D240" s="3"/>
     </row>
-    <row r="241" spans="4:4" ht="15.75" customHeight="1">
+    <row r="241" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D241" s="3"/>
     </row>
-    <row r="242" spans="4:4" ht="15.75" customHeight="1">
+    <row r="242" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D242" s="3"/>
     </row>
-    <row r="243" spans="4:4" ht="15.75" customHeight="1">
+    <row r="243" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D243" s="3"/>
     </row>
-    <row r="244" spans="4:4" ht="15.75" customHeight="1">
+    <row r="244" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D244" s="3"/>
     </row>
-    <row r="245" spans="4:4" ht="15.75" customHeight="1">
+    <row r="245" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D245" s="3"/>
     </row>
-    <row r="246" spans="4:4" ht="15.75" customHeight="1">
+    <row r="246" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D246" s="3"/>
     </row>
-    <row r="247" spans="4:4" ht="15.75" customHeight="1">
+    <row r="247" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D247" s="3"/>
     </row>
-    <row r="248" spans="4:4" ht="15.75" customHeight="1">
+    <row r="248" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D248" s="3"/>
     </row>
-    <row r="249" spans="4:4" ht="15.75" customHeight="1">
+    <row r="249" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D249" s="3"/>
     </row>
-    <row r="250" spans="4:4" ht="15.75" customHeight="1">
+    <row r="250" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D250" s="3"/>
     </row>
-    <row r="251" spans="4:4" ht="15.75" customHeight="1">
+    <row r="251" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D251" s="3"/>
     </row>
-    <row r="252" spans="4:4" ht="15.75" customHeight="1">
+    <row r="252" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D252" s="3"/>
     </row>
-    <row r="253" spans="4:4" ht="15.75" customHeight="1">
+    <row r="253" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D253" s="3"/>
     </row>
-    <row r="254" spans="4:4" ht="15.75" customHeight="1">
+    <row r="254" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D254" s="3"/>
     </row>
-    <row r="255" spans="4:4" ht="15.75" customHeight="1">
+    <row r="255" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D255" s="3"/>
     </row>
-    <row r="256" spans="4:4" ht="15.75" customHeight="1">
+    <row r="256" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D256" s="3"/>
     </row>
-    <row r="257" spans="4:4" ht="15.75" customHeight="1">
+    <row r="257" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D257" s="3"/>
     </row>
-    <row r="258" spans="4:4" ht="15.75" customHeight="1">
+    <row r="258" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D258" s="3"/>
     </row>
-    <row r="259" spans="4:4" ht="15.75" customHeight="1">
+    <row r="259" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D259" s="3"/>
     </row>
-    <row r="260" spans="4:4" ht="15.75" customHeight="1">
+    <row r="260" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D260" s="3"/>
     </row>
-    <row r="261" spans="4:4" ht="15.75" customHeight="1">
+    <row r="261" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D261" s="3"/>
     </row>
-    <row r="262" spans="4:4" ht="15.75" customHeight="1">
+    <row r="262" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D262" s="3"/>
     </row>
-    <row r="263" spans="4:4" ht="15.75" customHeight="1">
+    <row r="263" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D263" s="3"/>
     </row>
-    <row r="264" spans="4:4" ht="15.75" customHeight="1">
+    <row r="264" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D264" s="3"/>
     </row>
-    <row r="265" spans="4:4" ht="15.75" customHeight="1">
+    <row r="265" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D265" s="3"/>
     </row>
-    <row r="266" spans="4:4" ht="15.75" customHeight="1">
+    <row r="266" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D266" s="3"/>
     </row>
-    <row r="267" spans="4:4" ht="15.75" customHeight="1">
+    <row r="267" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D267" s="3"/>
     </row>
-    <row r="268" spans="4:4" ht="15.75" customHeight="1">
+    <row r="268" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D268" s="3"/>
     </row>
-    <row r="269" spans="4:4" ht="15.75" customHeight="1">
+    <row r="269" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D269" s="3"/>
     </row>
-    <row r="270" spans="4:4" ht="15.75" customHeight="1">
+    <row r="270" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D270" s="3"/>
     </row>
-    <row r="271" spans="4:4" ht="15.75" customHeight="1">
+    <row r="271" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D271" s="3"/>
     </row>
-    <row r="272" spans="4:4" ht="15.75" customHeight="1">
+    <row r="272" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D272" s="3"/>
     </row>
-    <row r="273" spans="4:4" ht="15.75" customHeight="1">
+    <row r="273" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D273" s="3"/>
     </row>
-    <row r="274" spans="4:4" ht="15.75" customHeight="1">
+    <row r="274" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D274" s="3"/>
     </row>
-    <row r="275" spans="4:4" ht="15.75" customHeight="1">
+    <row r="275" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D275" s="3"/>
     </row>
-    <row r="276" spans="4:4" ht="15.75" customHeight="1">
+    <row r="276" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D276" s="3"/>
     </row>
-    <row r="277" spans="4:4" ht="15.75" customHeight="1">
+    <row r="277" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D277" s="3"/>
     </row>
-    <row r="278" spans="4:4" ht="15.75" customHeight="1">
+    <row r="278" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D278" s="3"/>
     </row>
-    <row r="279" spans="4:4" ht="15.75" customHeight="1">
+    <row r="279" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D279" s="3"/>
     </row>
-    <row r="280" spans="4:4" ht="15.75" customHeight="1">
+    <row r="280" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D280" s="3"/>
     </row>
-    <row r="281" spans="4:4" ht="15.75" customHeight="1">
+    <row r="281" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D281" s="3"/>
     </row>
-    <row r="282" spans="4:4" ht="15.75" customHeight="1">
+    <row r="282" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D282" s="3"/>
     </row>
-    <row r="283" spans="4:4" ht="15.75" customHeight="1">
+    <row r="283" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D283" s="3"/>
     </row>
-    <row r="284" spans="4:4" ht="15.75" customHeight="1">
+    <row r="284" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D284" s="3"/>
     </row>
-    <row r="285" spans="4:4" ht="15.75" customHeight="1">
+    <row r="285" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D285" s="3"/>
     </row>
-    <row r="286" spans="4:4" ht="15.75" customHeight="1">
+    <row r="286" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D286" s="3"/>
     </row>
-    <row r="287" spans="4:4" ht="15.75" customHeight="1">
+    <row r="287" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D287" s="3"/>
     </row>
-    <row r="288" spans="4:4" ht="15.75" customHeight="1">
+    <row r="288" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D288" s="3"/>
     </row>
-    <row r="289" spans="4:4" ht="15.75" customHeight="1">
+    <row r="289" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D289" s="3"/>
     </row>
-    <row r="290" spans="4:4" ht="15.75" customHeight="1">
+    <row r="290" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D290" s="3"/>
     </row>
-    <row r="291" spans="4:4" ht="15.75" customHeight="1">
+    <row r="291" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D291" s="3"/>
     </row>
-    <row r="292" spans="4:4" ht="15.75" customHeight="1">
+    <row r="292" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D292" s="3"/>
     </row>
-    <row r="293" spans="4:4" ht="15.75" customHeight="1">
+    <row r="293" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D293" s="3"/>
     </row>
-    <row r="294" spans="4:4" ht="15.75" customHeight="1">
+    <row r="294" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D294" s="3"/>
     </row>
-    <row r="295" spans="4:4" ht="15.75" customHeight="1">
+    <row r="295" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D295" s="3"/>
     </row>
-    <row r="296" spans="4:4" ht="15.75" customHeight="1">
+    <row r="296" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D296" s="3"/>
     </row>
-    <row r="297" spans="4:4" ht="15.75" customHeight="1">
+    <row r="297" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D297" s="3"/>
     </row>
-    <row r="298" spans="4:4" ht="15.75" customHeight="1">
+    <row r="298" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D298" s="3"/>
     </row>
-    <row r="299" spans="4:4" ht="15.75" customHeight="1">
+    <row r="299" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D299" s="3"/>
     </row>
-    <row r="300" spans="4:4" ht="15.75" customHeight="1">
+    <row r="300" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D300" s="3"/>
     </row>
-    <row r="301" spans="4:4" ht="15.75" customHeight="1">
+    <row r="301" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D301" s="3"/>
     </row>
-    <row r="302" spans="4:4" ht="15.75" customHeight="1">
+    <row r="302" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D302" s="3"/>
     </row>
-    <row r="303" spans="4:4" ht="15.75" customHeight="1">
+    <row r="303" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D303" s="3"/>
     </row>
-    <row r="304" spans="4:4" ht="15.75" customHeight="1">
+    <row r="304" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D304" s="3"/>
     </row>
-    <row r="305" spans="4:4" ht="15.75" customHeight="1">
+    <row r="305" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D305" s="3"/>
     </row>
-    <row r="306" spans="4:4" ht="15.75" customHeight="1">
+    <row r="306" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D306" s="3"/>
     </row>
-    <row r="307" spans="4:4" ht="15.75" customHeight="1">
+    <row r="307" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D307" s="3"/>
     </row>
-    <row r="308" spans="4:4" ht="15.75" customHeight="1">
+    <row r="308" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D308" s="3"/>
     </row>
-    <row r="309" spans="4:4" ht="15.75" customHeight="1">
+    <row r="309" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D309" s="3"/>
     </row>
-    <row r="310" spans="4:4" ht="15.75" customHeight="1">
+    <row r="310" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D310" s="3"/>
     </row>
-    <row r="311" spans="4:4" ht="15.75" customHeight="1">
+    <row r="311" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D311" s="3"/>
     </row>
-    <row r="312" spans="4:4" ht="15.75" customHeight="1">
+    <row r="312" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D312" s="3"/>
     </row>
-    <row r="313" spans="4:4" ht="15.75" customHeight="1">
+    <row r="313" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D313" s="3"/>
     </row>
-    <row r="314" spans="4:4" ht="15.75" customHeight="1">
+    <row r="314" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D314" s="3"/>
     </row>
-    <row r="315" spans="4:4" ht="15.75" customHeight="1">
+    <row r="315" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D315" s="3"/>
     </row>
-    <row r="316" spans="4:4" ht="15.75" customHeight="1">
+    <row r="316" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D316" s="3"/>
     </row>
-    <row r="317" spans="4:4" ht="15.75" customHeight="1">
+    <row r="317" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D317" s="3"/>
     </row>
-    <row r="318" spans="4:4" ht="15.75" customHeight="1">
+    <row r="318" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D318" s="3"/>
     </row>
-    <row r="319" spans="4:4" ht="15.75" customHeight="1">
+    <row r="319" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D319" s="3"/>
     </row>
-    <row r="320" spans="4:4" ht="15.75" customHeight="1">
+    <row r="320" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D320" s="3"/>
     </row>
-    <row r="321" spans="4:4" ht="15.75" customHeight="1">
+    <row r="321" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D321" s="3"/>
     </row>
-    <row r="322" spans="4:4" ht="15.75" customHeight="1">
+    <row r="322" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D322" s="3"/>
     </row>
-    <row r="323" spans="4:4" ht="15.75" customHeight="1">
+    <row r="323" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D323" s="3"/>
     </row>
-    <row r="324" spans="4:4" ht="15.75" customHeight="1">
+    <row r="324" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D324" s="3"/>
     </row>
-    <row r="325" spans="4:4" ht="15.75" customHeight="1">
+    <row r="325" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D325" s="3"/>
     </row>
-    <row r="326" spans="4:4" ht="15.75" customHeight="1">
+    <row r="326" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D326" s="3"/>
     </row>
-    <row r="327" spans="4:4" ht="15.75" customHeight="1">
+    <row r="327" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D327" s="3"/>
     </row>
-    <row r="328" spans="4:4" ht="15.75" customHeight="1">
+    <row r="328" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D328" s="3"/>
     </row>
-    <row r="329" spans="4:4" ht="15.75" customHeight="1">
+    <row r="329" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D329" s="3"/>
     </row>
-    <row r="330" spans="4:4" ht="15.75" customHeight="1">
+    <row r="330" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D330" s="3"/>
     </row>
-    <row r="331" spans="4:4" ht="15.75" customHeight="1">
+    <row r="331" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D331" s="3"/>
     </row>
-    <row r="332" spans="4:4" ht="15.75" customHeight="1">
+    <row r="332" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D332" s="3"/>
     </row>
-    <row r="333" spans="4:4" ht="15.75" customHeight="1">
+    <row r="333" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D333" s="3"/>
     </row>
-    <row r="334" spans="4:4" ht="15.75" customHeight="1">
+    <row r="334" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D334" s="3"/>
     </row>
-    <row r="335" spans="4:4" ht="15.75" customHeight="1">
+    <row r="335" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D335" s="3"/>
     </row>
-    <row r="336" spans="4:4" ht="15.75" customHeight="1">
+    <row r="336" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D336" s="3"/>
     </row>
-    <row r="337" spans="4:4" ht="15.75" customHeight="1">
+    <row r="337" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D337" s="3"/>
     </row>
-    <row r="338" spans="4:4" ht="15.75" customHeight="1">
+    <row r="338" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D338" s="3"/>
     </row>
-    <row r="339" spans="4:4" ht="15.75" customHeight="1">
+    <row r="339" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D339" s="3"/>
     </row>
-    <row r="340" spans="4:4" ht="15.75" customHeight="1">
+    <row r="340" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D340" s="3"/>
     </row>
-    <row r="341" spans="4:4" ht="15.75" customHeight="1">
+    <row r="341" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D341" s="3"/>
     </row>
-    <row r="342" spans="4:4" ht="15.75" customHeight="1">
+    <row r="342" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D342" s="3"/>
     </row>
-    <row r="343" spans="4:4" ht="15.75" customHeight="1">
+    <row r="343" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D343" s="3"/>
     </row>
-    <row r="344" spans="4:4" ht="15.75" customHeight="1">
+    <row r="344" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D344" s="3"/>
     </row>
-    <row r="345" spans="4:4" ht="15.75" customHeight="1">
+    <row r="345" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D345" s="3"/>
     </row>
-    <row r="346" spans="4:4" ht="15.75" customHeight="1">
+    <row r="346" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D346" s="3"/>
     </row>
-    <row r="347" spans="4:4" ht="15.75" customHeight="1">
+    <row r="347" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D347" s="3"/>
     </row>
-    <row r="348" spans="4:4" ht="15.75" customHeight="1">
+    <row r="348" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D348" s="3"/>
     </row>
-    <row r="349" spans="4:4" ht="15.75" customHeight="1">
+    <row r="349" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D349" s="3"/>
     </row>
-    <row r="350" spans="4:4" ht="15.75" customHeight="1">
+    <row r="350" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D350" s="3"/>
     </row>
-    <row r="351" spans="4:4" ht="15.75" customHeight="1">
+    <row r="351" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D351" s="3"/>
     </row>
-    <row r="352" spans="4:4" ht="15.75" customHeight="1">
+    <row r="352" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D352" s="3"/>
     </row>
-    <row r="353" spans="4:4" ht="15.75" customHeight="1">
+    <row r="353" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D353" s="3"/>
     </row>
-    <row r="354" spans="4:4" ht="15.75" customHeight="1">
+    <row r="354" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D354" s="3"/>
     </row>
-    <row r="355" spans="4:4" ht="15.75" customHeight="1">
+    <row r="355" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D355" s="3"/>
     </row>
-    <row r="356" spans="4:4" ht="15.75" customHeight="1">
+    <row r="356" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D356" s="3"/>
     </row>
-    <row r="357" spans="4:4" ht="15.75" customHeight="1">
+    <row r="357" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D357" s="3"/>
     </row>
-    <row r="358" spans="4:4" ht="15.75" customHeight="1">
+    <row r="358" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D358" s="3"/>
     </row>
-    <row r="359" spans="4:4" ht="15.75" customHeight="1">
+    <row r="359" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D359" s="3"/>
     </row>
-    <row r="360" spans="4:4" ht="15.75" customHeight="1">
+    <row r="360" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D360" s="3"/>
     </row>
-    <row r="361" spans="4:4" ht="15.75" customHeight="1">
+    <row r="361" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D361" s="3"/>
     </row>
-    <row r="362" spans="4:4" ht="15.75" customHeight="1">
+    <row r="362" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D362" s="3"/>
     </row>
-    <row r="363" spans="4:4" ht="15.75" customHeight="1">
+    <row r="363" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D363" s="3"/>
     </row>
-    <row r="364" spans="4:4" ht="15.75" customHeight="1">
+    <row r="364" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D364" s="3"/>
     </row>
-    <row r="365" spans="4:4" ht="15.75" customHeight="1">
+    <row r="365" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D365" s="3"/>
     </row>
-    <row r="366" spans="4:4" ht="15.75" customHeight="1">
+    <row r="366" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D366" s="3"/>
     </row>
-    <row r="367" spans="4:4" ht="15.75" customHeight="1">
+    <row r="367" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D367" s="3"/>
     </row>
-    <row r="368" spans="4:4" ht="15.75" customHeight="1">
+    <row r="368" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D368" s="3"/>
     </row>
-    <row r="369" spans="4:4" ht="15.75" customHeight="1">
+    <row r="369" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D369" s="3"/>
     </row>
-    <row r="370" spans="4:4" ht="15.75" customHeight="1">
+    <row r="370" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D370" s="3"/>
     </row>
-    <row r="371" spans="4:4" ht="15.75" customHeight="1">
+    <row r="371" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D371" s="3"/>
     </row>
-    <row r="372" spans="4:4" ht="15.75" customHeight="1">
+    <row r="372" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D372" s="3"/>
     </row>
-    <row r="373" spans="4:4" ht="15.75" customHeight="1">
+    <row r="373" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D373" s="3"/>
     </row>
-    <row r="374" spans="4:4" ht="15.75" customHeight="1">
+    <row r="374" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D374" s="3"/>
     </row>
-    <row r="375" spans="4:4" ht="15.75" customHeight="1">
+    <row r="375" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D375" s="3"/>
     </row>
-    <row r="376" spans="4:4" ht="15.75" customHeight="1">
+    <row r="376" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D376" s="3"/>
     </row>
-    <row r="377" spans="4:4" ht="15.75" customHeight="1">
+    <row r="377" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D377" s="3"/>
     </row>
-    <row r="378" spans="4:4" ht="15.75" customHeight="1">
+    <row r="378" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D378" s="3"/>
     </row>
-    <row r="379" spans="4:4" ht="15.75" customHeight="1">
+    <row r="379" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D379" s="3"/>
     </row>
-    <row r="380" spans="4:4" ht="15.75" customHeight="1">
+    <row r="380" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D380" s="3"/>
     </row>
-    <row r="381" spans="4:4" ht="15.75" customHeight="1">
+    <row r="381" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D381" s="3"/>
     </row>
-    <row r="382" spans="4:4" ht="15.75" customHeight="1">
+    <row r="382" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D382" s="3"/>
     </row>
-    <row r="383" spans="4:4" ht="15.75" customHeight="1">
+    <row r="383" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D383" s="3"/>
     </row>
-    <row r="384" spans="4:4" ht="15.75" customHeight="1">
+    <row r="384" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D384" s="3"/>
     </row>
-    <row r="385" spans="4:4" ht="15.75" customHeight="1">
+    <row r="385" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D385" s="3"/>
     </row>
-    <row r="386" spans="4:4" ht="15.75" customHeight="1">
+    <row r="386" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D386" s="3"/>
     </row>
-    <row r="387" spans="4:4" ht="15.75" customHeight="1">
+    <row r="387" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D387" s="3"/>
     </row>
-    <row r="388" spans="4:4" ht="15.75" customHeight="1">
+    <row r="388" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D388" s="3"/>
     </row>
-    <row r="389" spans="4:4" ht="15.75" customHeight="1">
+    <row r="389" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D389" s="3"/>
     </row>
-    <row r="390" spans="4:4" ht="15.75" customHeight="1">
+    <row r="390" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D390" s="3"/>
     </row>
-    <row r="391" spans="4:4" ht="15.75" customHeight="1">
+    <row r="391" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D391" s="3"/>
     </row>
-    <row r="392" spans="4:4" ht="15.75" customHeight="1">
+    <row r="392" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D392" s="3"/>
     </row>
-    <row r="393" spans="4:4" ht="15.75" customHeight="1">
+    <row r="393" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D393" s="3"/>
     </row>
-    <row r="394" spans="4:4" ht="15.75" customHeight="1">
+    <row r="394" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D394" s="3"/>
     </row>
-    <row r="395" spans="4:4" ht="15.75" customHeight="1">
+    <row r="395" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D395" s="3"/>
     </row>
-    <row r="396" spans="4:4" ht="15.75" customHeight="1">
+    <row r="396" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D396" s="3"/>
     </row>
-    <row r="397" spans="4:4" ht="15.75" customHeight="1">
+    <row r="397" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D397" s="3"/>
     </row>
-    <row r="398" spans="4:4" ht="15.75" customHeight="1">
+    <row r="398" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D398" s="3"/>
     </row>
-    <row r="399" spans="4:4" ht="15.75" customHeight="1">
+    <row r="399" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D399" s="3"/>
     </row>
-    <row r="400" spans="4:4" ht="15.75" customHeight="1">
+    <row r="400" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D400" s="3"/>
     </row>
-    <row r="401" spans="4:4" ht="15.75" customHeight="1">
+    <row r="401" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D401" s="3"/>
     </row>
-    <row r="402" spans="4:4" ht="15.75" customHeight="1">
+    <row r="402" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D402" s="3"/>
     </row>
-    <row r="403" spans="4:4" ht="15.75" customHeight="1">
+    <row r="403" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D403" s="3"/>
     </row>
-    <row r="404" spans="4:4" ht="15.75" customHeight="1">
+    <row r="404" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D404" s="3"/>
     </row>
-    <row r="405" spans="4:4" ht="15.75" customHeight="1">
+    <row r="405" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D405" s="3"/>
     </row>
-    <row r="406" spans="4:4" ht="15.75" customHeight="1">
+    <row r="406" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D406" s="3"/>
     </row>
-    <row r="407" spans="4:4" ht="15.75" customHeight="1">
+    <row r="407" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D407" s="3"/>
     </row>
-    <row r="408" spans="4:4" ht="15.75" customHeight="1">
+    <row r="408" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D408" s="3"/>
     </row>
-    <row r="409" spans="4:4" ht="15.75" customHeight="1">
+    <row r="409" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D409" s="3"/>
     </row>
-    <row r="410" spans="4:4" ht="15.75" customHeight="1">
+    <row r="410" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D410" s="3"/>
     </row>
-    <row r="411" spans="4:4" ht="15.75" customHeight="1">
+    <row r="411" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D411" s="3"/>
     </row>
-    <row r="412" spans="4:4" ht="15.75" customHeight="1">
+    <row r="412" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D412" s="3"/>
     </row>
-    <row r="413" spans="4:4" ht="15.75" customHeight="1">
+    <row r="413" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D413" s="3"/>
     </row>
-    <row r="414" spans="4:4" ht="15.75" customHeight="1">
+    <row r="414" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D414" s="3"/>
     </row>
-    <row r="415" spans="4:4" ht="15.75" customHeight="1">
+    <row r="415" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D415" s="3"/>
     </row>
-    <row r="416" spans="4:4" ht="15.75" customHeight="1">
+    <row r="416" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D416" s="3"/>
     </row>
-    <row r="417" spans="4:4" ht="15.75" customHeight="1">
+    <row r="417" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D417" s="3"/>
     </row>
-    <row r="418" spans="4:4" ht="15.75" customHeight="1">
+    <row r="418" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D418" s="3"/>
     </row>
-    <row r="419" spans="4:4" ht="15.75" customHeight="1">
+    <row r="419" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D419" s="3"/>
     </row>
-    <row r="420" spans="4:4" ht="15.75" customHeight="1">
+    <row r="420" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D420" s="3"/>
     </row>
-    <row r="421" spans="4:4" ht="15.75" customHeight="1">
+    <row r="421" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D421" s="3"/>
     </row>
-    <row r="422" spans="4:4" ht="15.75" customHeight="1">
+    <row r="422" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D422" s="3"/>
     </row>
-    <row r="423" spans="4:4" ht="15.75" customHeight="1">
+    <row r="423" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D423" s="3"/>
     </row>
-    <row r="424" spans="4:4" ht="15.75" customHeight="1">
+    <row r="424" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D424" s="3"/>
     </row>
-    <row r="425" spans="4:4" ht="15.75" customHeight="1">
+    <row r="425" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D425" s="3"/>
     </row>
-    <row r="426" spans="4:4" ht="15.75" customHeight="1">
+    <row r="426" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D426" s="3"/>
     </row>
-    <row r="427" spans="4:4" ht="15.75" customHeight="1">
+    <row r="427" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D427" s="3"/>
     </row>
-    <row r="428" spans="4:4" ht="15.75" customHeight="1">
+    <row r="428" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D428" s="3"/>
     </row>
-    <row r="429" spans="4:4" ht="15.75" customHeight="1">
+    <row r="429" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D429" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow empty for each language.
</commit_message>
<xml_diff>
--- a/LanguageParser.xlsx
+++ b/LanguageParser.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukelin/Documents/WorkSpaceLuke/LanguageParser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukelin/Documents/WorkSpaceLuke/Python/LanguageParser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -90,6 +90,30 @@
   </si>
   <si>
     <t>名字是%S%, 年龄是%D%</t>
+  </si>
+  <si>
+    <t>ANDROID</t>
+  </si>
+  <si>
+    <t>IOS</t>
+  </si>
+  <si>
+    <t>account_for_android_string</t>
+  </si>
+  <si>
+    <t>account_for_ios_string</t>
+  </si>
+  <si>
+    <t>Android String</t>
+  </si>
+  <si>
+    <t>iOS String</t>
+  </si>
+  <si>
+    <t>Android String fr</t>
+  </si>
+  <si>
+    <t>iOS String zh</t>
   </si>
 </sst>
 </file>
@@ -487,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA429"/>
+  <dimension ref="A1:AA428"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -609,10 +633,33 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D6" s="3"/>
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D7" s="3"/>
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D8" s="3"/>
@@ -620,9 +667,6 @@
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D10" s="3"/>
-    </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D11" s="3"/>
     </row>
@@ -1876,9 +1920,6 @@
     </row>
     <row r="428" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D428" s="3"/>
-    </row>
-    <row r="429" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D429" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>